<commit_message>
Removing old files and updating workflow
</commit_message>
<xml_diff>
--- a/data/Ranked_Contacts.xlsx
+++ b/data/Ranked_Contacts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="102">
   <si>
     <t>Rank</t>
   </si>
@@ -260,36 +260,6 @@
   </si>
   <si>
     <t>MD</t>
-  </si>
-  <si>
-    <t>20001</t>
-  </si>
-  <si>
-    <t>22201</t>
-  </si>
-  <si>
-    <t>20877</t>
-  </si>
-  <si>
-    <t>20814</t>
-  </si>
-  <si>
-    <t>20011</t>
-  </si>
-  <si>
-    <t>22030</t>
-  </si>
-  <si>
-    <t>20852</t>
-  </si>
-  <si>
-    <t>20910</t>
-  </si>
-  <si>
-    <t>22046</t>
-  </si>
-  <si>
-    <t>22314</t>
   </si>
   <si>
     <t>Primary Care</t>
@@ -761,11 +731,11 @@
       <c r="E2" t="s">
         <v>79</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>20001</v>
+      </c>
+      <c r="G2" t="s">
         <v>82</v>
-      </c>
-      <c r="G2" t="s">
-        <v>92</v>
       </c>
       <c r="H2">
         <v>40.69298</v>
@@ -774,7 +744,7 @@
         <v>-89.407219</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -793,14 +763,14 @@
       <c r="E3" t="s">
         <v>79</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>20001</v>
+      </c>
+      <c r="G3" t="s">
         <v>82</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>92</v>
-      </c>
-      <c r="J3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -819,14 +789,14 @@
       <c r="E4" t="s">
         <v>80</v>
       </c>
-      <c r="F4" t="s">
-        <v>83</v>
+      <c r="F4">
+        <v>22201</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="J4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -845,14 +815,14 @@
       <c r="E5" t="s">
         <v>81</v>
       </c>
-      <c r="F5" t="s">
-        <v>84</v>
+      <c r="F5">
+        <v>20877</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="J5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -871,11 +841,11 @@
       <c r="E6" t="s">
         <v>81</v>
       </c>
-      <c r="F6" t="s">
-        <v>85</v>
+      <c r="F6">
+        <v>20814</v>
       </c>
       <c r="G6" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H6">
         <v>39.0069593</v>
@@ -884,7 +854,7 @@
         <v>-77.096464</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -903,14 +873,14 @@
       <c r="E7" t="s">
         <v>79</v>
       </c>
-      <c r="F7" t="s">
-        <v>86</v>
+      <c r="F7">
+        <v>20011</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -929,11 +899,11 @@
       <c r="E8" t="s">
         <v>80</v>
       </c>
-      <c r="F8" t="s">
-        <v>87</v>
+      <c r="F8">
+        <v>22030</v>
       </c>
       <c r="G8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H8">
         <v>38.8490309</v>
@@ -942,7 +912,7 @@
         <v>-77.3212525</v>
       </c>
       <c r="J8" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -961,11 +931,11 @@
       <c r="E9" t="s">
         <v>80</v>
       </c>
-      <c r="F9" t="s">
-        <v>87</v>
+      <c r="F9">
+        <v>22030</v>
       </c>
       <c r="G9" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H9">
         <v>38.8490309</v>
@@ -974,7 +944,7 @@
         <v>-77.3212525</v>
       </c>
       <c r="J9" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -993,14 +963,14 @@
       <c r="E10" t="s">
         <v>81</v>
       </c>
-      <c r="F10" t="s">
-        <v>88</v>
+      <c r="F10">
+        <v>20852</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="J10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1019,11 +989,11 @@
       <c r="E11" t="s">
         <v>81</v>
       </c>
-      <c r="F11" t="s">
-        <v>89</v>
+      <c r="F11">
+        <v>20910</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H11">
         <v>38.9920956</v>
@@ -1032,7 +1002,7 @@
         <v>-77.090879</v>
       </c>
       <c r="J11" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1051,11 +1021,11 @@
       <c r="E12" t="s">
         <v>81</v>
       </c>
-      <c r="F12" t="s">
-        <v>85</v>
+      <c r="F12">
+        <v>20814</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="H12">
         <v>39.0069593</v>
@@ -1064,7 +1034,7 @@
         <v>-77.096464</v>
       </c>
       <c r="J12" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1083,14 +1053,14 @@
       <c r="E13" t="s">
         <v>79</v>
       </c>
-      <c r="F13" t="s">
-        <v>82</v>
+      <c r="F13">
+        <v>20001</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J13" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1109,14 +1079,14 @@
       <c r="E14" t="s">
         <v>80</v>
       </c>
-      <c r="F14" t="s">
-        <v>83</v>
+      <c r="F14">
+        <v>22201</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J14" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1135,14 +1105,14 @@
       <c r="E15" t="s">
         <v>80</v>
       </c>
-      <c r="F15" t="s">
-        <v>83</v>
+      <c r="F15">
+        <v>22201</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J15" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1161,11 +1131,11 @@
       <c r="E16" t="s">
         <v>81</v>
       </c>
-      <c r="F16" t="s">
-        <v>85</v>
+      <c r="F16">
+        <v>20814</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="H16">
         <v>39.0069593</v>
@@ -1174,7 +1144,7 @@
         <v>-77.096464</v>
       </c>
       <c r="J16" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1193,11 +1163,11 @@
       <c r="E17" t="s">
         <v>81</v>
       </c>
-      <c r="F17" t="s">
-        <v>89</v>
+      <c r="F17">
+        <v>20910</v>
       </c>
       <c r="G17" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="H17">
         <v>38.9920956</v>
@@ -1206,7 +1176,7 @@
         <v>-77.090879</v>
       </c>
       <c r="J17" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1225,14 +1195,14 @@
       <c r="E18" t="s">
         <v>79</v>
       </c>
-      <c r="F18" t="s">
-        <v>86</v>
+      <c r="F18">
+        <v>20011</v>
       </c>
       <c r="G18" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J18" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1251,14 +1221,14 @@
       <c r="E19" t="s">
         <v>79</v>
       </c>
-      <c r="F19" t="s">
-        <v>86</v>
+      <c r="F19">
+        <v>20011</v>
       </c>
       <c r="G19" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J19" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1277,11 +1247,11 @@
       <c r="E20" t="s">
         <v>81</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20">
+        <v>20814</v>
+      </c>
+      <c r="G20" t="s">
         <v>85</v>
-      </c>
-      <c r="G20" t="s">
-        <v>95</v>
       </c>
       <c r="H20">
         <v>39.0069593</v>
@@ -1290,7 +1260,7 @@
         <v>-77.096464</v>
       </c>
       <c r="J20" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1309,14 +1279,14 @@
       <c r="E21" t="s">
         <v>79</v>
       </c>
-      <c r="F21" t="s">
-        <v>82</v>
+      <c r="F21">
+        <v>20001</v>
       </c>
       <c r="G21" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J21" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1335,11 +1305,11 @@
       <c r="E22" t="s">
         <v>80</v>
       </c>
-      <c r="F22" t="s">
-        <v>87</v>
+      <c r="F22">
+        <v>22030</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H22">
         <v>38.8490309</v>
@@ -1348,7 +1318,7 @@
         <v>-77.3212525</v>
       </c>
       <c r="J22" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1367,11 +1337,11 @@
       <c r="E23" t="s">
         <v>81</v>
       </c>
-      <c r="F23" t="s">
-        <v>85</v>
+      <c r="F23">
+        <v>20814</v>
       </c>
       <c r="G23" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H23">
         <v>39.0069593</v>
@@ -1380,7 +1350,7 @@
         <v>-77.096464</v>
       </c>
       <c r="J23" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1399,11 +1369,11 @@
       <c r="E24" t="s">
         <v>81</v>
       </c>
-      <c r="F24" t="s">
-        <v>85</v>
+      <c r="F24">
+        <v>20814</v>
       </c>
       <c r="G24" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H24">
         <v>39.0069593</v>
@@ -1412,7 +1382,7 @@
         <v>-77.096464</v>
       </c>
       <c r="J24" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1431,11 +1401,11 @@
       <c r="E25" t="s">
         <v>81</v>
       </c>
-      <c r="F25" t="s">
-        <v>89</v>
+      <c r="F25">
+        <v>20910</v>
       </c>
       <c r="G25" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H25">
         <v>38.9920956</v>
@@ -1444,7 +1414,7 @@
         <v>-77.090879</v>
       </c>
       <c r="J25" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1463,11 +1433,11 @@
       <c r="E26" t="s">
         <v>81</v>
       </c>
-      <c r="F26" t="s">
-        <v>85</v>
+      <c r="F26">
+        <v>20814</v>
       </c>
       <c r="G26" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H26">
         <v>39.0069593</v>
@@ -1476,7 +1446,7 @@
         <v>-77.096464</v>
       </c>
       <c r="J26" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1495,11 +1465,11 @@
       <c r="E27" t="s">
         <v>81</v>
       </c>
-      <c r="F27" t="s">
-        <v>89</v>
+      <c r="F27">
+        <v>20910</v>
       </c>
       <c r="G27" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H27">
         <v>38.9920956</v>
@@ -1508,7 +1478,7 @@
         <v>-77.090879</v>
       </c>
       <c r="J27" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1527,14 +1497,14 @@
       <c r="E28" t="s">
         <v>81</v>
       </c>
-      <c r="F28" t="s">
-        <v>84</v>
+      <c r="F28">
+        <v>20877</v>
       </c>
       <c r="G28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="J28" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1553,11 +1523,11 @@
       <c r="E29" t="s">
         <v>80</v>
       </c>
-      <c r="F29" t="s">
-        <v>90</v>
+      <c r="F29">
+        <v>22046</v>
       </c>
       <c r="G29" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H29">
         <v>38.894131</v>
@@ -1566,7 +1536,7 @@
         <v>-77.18182</v>
       </c>
       <c r="J29" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1585,14 +1555,14 @@
       <c r="E30" t="s">
         <v>81</v>
       </c>
-      <c r="F30" t="s">
-        <v>88</v>
+      <c r="F30">
+        <v>20852</v>
       </c>
       <c r="G30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="J30" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1611,11 +1581,11 @@
       <c r="E31" t="s">
         <v>80</v>
       </c>
-      <c r="F31" t="s">
-        <v>90</v>
+      <c r="F31">
+        <v>22046</v>
       </c>
       <c r="G31" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H31">
         <v>38.894131</v>
@@ -1624,7 +1594,7 @@
         <v>-77.18182</v>
       </c>
       <c r="J31" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1643,11 +1613,11 @@
       <c r="E32" t="s">
         <v>80</v>
       </c>
-      <c r="F32" t="s">
-        <v>90</v>
+      <c r="F32">
+        <v>22046</v>
       </c>
       <c r="G32" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="H32">
         <v>38.894131</v>
@@ -1656,7 +1626,7 @@
         <v>-77.18182</v>
       </c>
       <c r="J32" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1675,14 +1645,14 @@
       <c r="E33" t="s">
         <v>79</v>
       </c>
-      <c r="F33" t="s">
-        <v>86</v>
+      <c r="F33">
+        <v>20011</v>
       </c>
       <c r="G33" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="J33" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1701,11 +1671,11 @@
       <c r="E34" t="s">
         <v>80</v>
       </c>
-      <c r="F34" t="s">
-        <v>90</v>
+      <c r="F34">
+        <v>22046</v>
       </c>
       <c r="G34" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="H34">
         <v>38.894131</v>
@@ -1714,7 +1684,7 @@
         <v>-77.18182</v>
       </c>
       <c r="J34" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1733,14 +1703,14 @@
       <c r="E35" t="s">
         <v>79</v>
       </c>
-      <c r="F35" t="s">
-        <v>82</v>
+      <c r="F35">
+        <v>20001</v>
       </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="J35" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1759,14 +1729,14 @@
       <c r="E36" t="s">
         <v>79</v>
       </c>
-      <c r="F36" t="s">
-        <v>82</v>
+      <c r="F36">
+        <v>20001</v>
       </c>
       <c r="G36" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="J36" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1785,14 +1755,14 @@
       <c r="E37" t="s">
         <v>79</v>
       </c>
-      <c r="F37" t="s">
-        <v>82</v>
+      <c r="F37">
+        <v>20001</v>
       </c>
       <c r="G37" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="J37" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1811,14 +1781,14 @@
       <c r="E38" t="s">
         <v>80</v>
       </c>
-      <c r="F38" t="s">
-        <v>83</v>
+      <c r="F38">
+        <v>22201</v>
       </c>
       <c r="G38" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="J38" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1837,11 +1807,11 @@
       <c r="E39" t="s">
         <v>80</v>
       </c>
-      <c r="F39" t="s">
-        <v>87</v>
+      <c r="F39">
+        <v>22030</v>
       </c>
       <c r="G39" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="H39">
         <v>38.8490309</v>
@@ -1850,7 +1820,7 @@
         <v>-77.3212525</v>
       </c>
       <c r="J39" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1869,11 +1839,11 @@
       <c r="E40" t="s">
         <v>80</v>
       </c>
-      <c r="F40" t="s">
-        <v>87</v>
+      <c r="F40">
+        <v>22030</v>
       </c>
       <c r="G40" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="H40">
         <v>38.8490309</v>
@@ -1882,7 +1852,7 @@
         <v>-77.3212525</v>
       </c>
       <c r="J40" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1901,14 +1871,14 @@
       <c r="E41" t="s">
         <v>80</v>
       </c>
-      <c r="F41" t="s">
-        <v>83</v>
+      <c r="F41">
+        <v>22201</v>
       </c>
       <c r="G41" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="J41" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1927,14 +1897,14 @@
       <c r="E42" t="s">
         <v>81</v>
       </c>
-      <c r="F42" t="s">
-        <v>84</v>
+      <c r="F42">
+        <v>20877</v>
       </c>
       <c r="G42" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J42" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1953,14 +1923,14 @@
       <c r="E43" t="s">
         <v>81</v>
       </c>
-      <c r="F43" t="s">
-        <v>88</v>
+      <c r="F43">
+        <v>20852</v>
       </c>
       <c r="G43" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J43" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1979,14 +1949,14 @@
       <c r="E44" t="s">
         <v>80</v>
       </c>
-      <c r="F44" t="s">
-        <v>83</v>
+      <c r="F44">
+        <v>22201</v>
       </c>
       <c r="G44" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J44" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2005,11 +1975,11 @@
       <c r="E45" t="s">
         <v>80</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45">
+        <v>22046</v>
+      </c>
+      <c r="G45" t="s">
         <v>90</v>
-      </c>
-      <c r="G45" t="s">
-        <v>100</v>
       </c>
       <c r="H45">
         <v>38.894131</v>
@@ -2018,7 +1988,7 @@
         <v>-77.18182</v>
       </c>
       <c r="J45" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2037,11 +2007,11 @@
       <c r="E46" t="s">
         <v>81</v>
       </c>
-      <c r="F46" t="s">
-        <v>89</v>
+      <c r="F46">
+        <v>20910</v>
       </c>
       <c r="G46" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H46">
         <v>38.9920956</v>
@@ -2050,7 +2020,7 @@
         <v>-77.090879</v>
       </c>
       <c r="J46" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2069,11 +2039,11 @@
       <c r="E47" t="s">
         <v>80</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47">
+        <v>22314</v>
+      </c>
+      <c r="G47" t="s">
         <v>91</v>
-      </c>
-      <c r="G47" t="s">
-        <v>101</v>
       </c>
       <c r="H47">
         <v>38.8310013</v>
@@ -2082,7 +2052,7 @@
         <v>-77.0660113</v>
       </c>
       <c r="J47" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2101,11 +2071,11 @@
       <c r="E48" t="s">
         <v>81</v>
       </c>
-      <c r="F48" t="s">
-        <v>89</v>
+      <c r="F48">
+        <v>20910</v>
       </c>
       <c r="G48" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H48">
         <v>38.9920956</v>
@@ -2114,7 +2084,7 @@
         <v>-77.090879</v>
       </c>
       <c r="J48" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2133,14 +2103,14 @@
       <c r="E49" t="s">
         <v>81</v>
       </c>
-      <c r="F49" t="s">
-        <v>84</v>
+      <c r="F49">
+        <v>20877</v>
       </c>
       <c r="G49" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="J49" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2159,14 +2129,14 @@
       <c r="E50" t="s">
         <v>80</v>
       </c>
-      <c r="F50" t="s">
-        <v>83</v>
+      <c r="F50">
+        <v>22201</v>
       </c>
       <c r="G50" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="J50" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2185,11 +2155,11 @@
       <c r="E51" t="s">
         <v>80</v>
       </c>
-      <c r="F51" t="s">
-        <v>87</v>
+      <c r="F51">
+        <v>22030</v>
       </c>
       <c r="G51" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H51">
         <v>38.8490309</v>
@@ -2198,7 +2168,7 @@
         <v>-77.3212525</v>
       </c>
       <c r="J51" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>